<commit_message>
Lesson Leaned and Conclusion
completed ReadMe and added additional graphics
</commit_message>
<xml_diff>
--- a/project_sql/query2_skills_of_high_paying_roles.xlsx
+++ b/project_sql/query2_skills_of_high_paying_roles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David Parker\Documents\Dave's Stuff\Data_Analysis\SQL_Project_Data_Job_Analysis\project_sql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{6675336B-3E54-4F8A-A222-61513E289864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5173D909-9234-42B7-B738-13AAB7C63F20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{8CB73127-223C-439F-B3D7-0913AA40423C}"/>
   </bookViews>
@@ -19,14 +19,14 @@
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="36" r:id="rId4"/>
-    <pivotCache cacheId="35" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="1" r:id="rId5"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="45">
   <si>
     <t>job_id</t>
   </si>
@@ -148,13 +148,19 @@
     <t xml:space="preserve"> salary_year_avg</t>
   </si>
   <si>
-    <t>Count of skills</t>
-  </si>
-  <si>
     <t>Average of salary_year_avg</t>
   </si>
   <si>
     <t># skills</t>
+  </si>
+  <si>
+    <t>Company Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Skills</t>
+  </si>
+  <si>
+    <t>SalaryYrAvg</t>
   </si>
 </sst>
 </file>
@@ -470,7 +476,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -585,6 +591,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="8" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -630,7 +645,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -638,9 +653,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -649,6 +661,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -694,24 +708,593 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="79">
+  <dxfs count="119">
     <dxf>
       <alignment horizontal="right"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <alignment horizontal="right"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="right"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="right"/>
     </dxf>
     <dxf>
@@ -742,6 +1325,9 @@
       <alignment horizontal="right"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="right"/>
     </dxf>
     <dxf>
@@ -761,138 +1347,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="right"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     </dxf>
     <dxf>
       <alignment horizontal="right"/>
@@ -3308,7 +3762,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D024F0B5-5A08-4AEC-AF7F-3CEC305933AA}" name="PivotTable45" cacheId="36" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D024F0B5-5A08-4AEC-AF7F-3CEC305933AA}" name="PivotTable45" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
   <location ref="A16:B23" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0"/>
@@ -3405,7 +3859,7 @@
     <dataField name="# skills" fld="5" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="41">
+    <format dxfId="95">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -3422,20 +3876,19 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{685A5C80-460B-4FB4-AE12-435FF5F463F8}" name="PivotTable26" cacheId="36" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9" fieldListSortAscending="1">
-  <location ref="A41:C93" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{685A5C80-460B-4FB4-AE12-435FF5F463F8}" name="PivotTable26" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="9" fieldListSortAscending="1">
+  <location ref="A41:C86" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="6">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="2">
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="1">
         <item x="0"/>
-        <item t="default"/>
       </items>
     </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField numFmtId="22" showAll="0"/>
-    <pivotField axis="axisRow" showAll="0" sortType="descending">
-      <items count="8">
+    <pivotField dataField="1" compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" numFmtId="22" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField name="Company Name" axis="axisRow" compact="0" outline="0" showAll="0" sortType="descending" defaultSubtotal="0">
+      <items count="7">
         <item x="1"/>
         <item x="2"/>
         <item x="0"/>
@@ -3443,7 +3896,6 @@
         <item x="5"/>
         <item x="6"/>
         <item x="4"/>
-        <item t="default"/>
       </items>
       <autoSortScope>
         <pivotArea dataOnly="0" outline="0" fieldPosition="0">
@@ -3455,8 +3907,8 @@
         </pivotArea>
       </autoSortScope>
     </pivotField>
-    <pivotField axis="axisRow" dataField="1" showAll="0" sortType="descending">
-      <items count="24">
+    <pivotField name=" Skills" axis="axisRow" compact="0" outline="0" showAll="0" sortType="descending" defaultSubtotal="0">
+      <items count="23">
         <item x="16"/>
         <item x="22"/>
         <item x="10"/>
@@ -3480,7 +3932,6 @@
         <item x="15"/>
         <item x="19"/>
         <item x="21"/>
-        <item t="default"/>
       </items>
       <autoSortScope>
         <pivotArea dataOnly="0" outline="0" fieldPosition="0">
@@ -3497,21 +3948,139 @@
     <field x="4"/>
     <field x="5"/>
   </rowFields>
-  <rowItems count="52">
+  <rowItems count="45">
     <i>
       <x v="2"/>
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="18"/>
+    </i>
+    <i r="1">
+      <x v="15"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="19"/>
+    </i>
+    <i r="1">
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x v="10"/>
+    </i>
+    <i>
+      <x/>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="14"/>
+    </i>
+    <i r="1">
+      <x v="13"/>
+    </i>
+    <i r="1">
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x v="15"/>
+    </i>
+    <i r="1">
+      <x v="10"/>
+    </i>
+    <i r="1">
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="17"/>
+    </i>
+    <i r="1">
+      <x v="16"/>
     </i>
     <i r="1">
       <x v="4"/>
     </i>
     <i r="1">
-      <x v="18"/>
+      <x v="20"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
     </i>
     <i r="1">
       <x v="15"/>
     </i>
+    <i>
+      <x v="3"/>
+      <x v="19"/>
+    </i>
     <i r="1">
+      <x v="11"/>
+    </i>
+    <i r="1">
+      <x v="10"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="15"/>
+    </i>
+    <i r="1">
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="6"/>
+      <x v="15"/>
+    </i>
+    <i r="1">
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="4"/>
+      <x v="21"/>
+    </i>
+    <i r="1">
+      <x v="12"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="15"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x v="22"/>
+    </i>
+    <i r="1">
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x v="10"/>
+    </i>
+    <i>
       <x v="5"/>
+      <x v="15"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
     </i>
     <i r="1">
       <x v="19"/>
@@ -3522,160 +4091,259 @@
     <i r="1">
       <x v="10"/>
     </i>
-    <i>
-      <x/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="14"/>
-    </i>
-    <i r="1">
-      <x v="13"/>
-    </i>
-    <i r="1">
-      <x v="8"/>
-    </i>
-    <i r="1">
-      <x v="15"/>
-    </i>
-    <i r="1">
-      <x v="10"/>
-    </i>
-    <i r="1">
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="17"/>
-    </i>
-    <i r="1">
-      <x v="16"/>
-    </i>
-    <i r="1">
-      <x v="4"/>
-    </i>
-    <i r="1">
-      <x v="20"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i r="1">
-      <x v="15"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="19"/>
-    </i>
-    <i r="1">
-      <x v="11"/>
-    </i>
-    <i r="1">
-      <x v="10"/>
-    </i>
-    <i r="1">
-      <x v="4"/>
-    </i>
-    <i r="1">
-      <x v="15"/>
-    </i>
-    <i r="1">
-      <x v="8"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i r="1">
-      <x v="15"/>
-    </i>
-    <i r="1">
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i r="1">
-      <x v="21"/>
-    </i>
-    <i r="1">
-      <x v="12"/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="4"/>
-    </i>
-    <i r="1">
-      <x v="15"/>
-    </i>
-    <i r="1">
-      <x v="7"/>
-    </i>
-    <i r="1">
-      <x v="22"/>
-    </i>
-    <i r="1">
-      <x v="8"/>
-    </i>
-    <i r="1">
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="15"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i r="1">
-      <x v="19"/>
-    </i>
-    <i r="1">
-      <x v="8"/>
-    </i>
-    <i r="1">
-      <x v="10"/>
-    </i>
   </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
+  <colItems count="1">
+    <i/>
   </colItems>
-  <dataFields count="2">
-    <dataField name="Average of salary_year_avg" fld="2" subtotal="average" baseField="5" baseItem="15" numFmtId="3"/>
-    <dataField name="Count of skills" fld="5" subtotal="count" showDataAs="runTotal" baseField="5" baseItem="4"/>
+  <dataFields count="1">
+    <dataField name="SalaryYrAvg" fld="2" subtotal="average" baseField="5" baseItem="15" numFmtId="164"/>
   </dataFields>
-  <formats count="1">
-    <format dxfId="52">
+  <formats count="23">
+    <format dxfId="96">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
+    <format dxfId="85">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="84">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="10"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="82">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" offset="IV256" fieldPosition="0">
+        <references count="1">
+          <reference field="4" count="1">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="80">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="5" count="1">
+            <x v="10"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="78">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="10"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="77">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" offset="IV256" fieldPosition="0">
+        <references count="1">
+          <reference field="4" count="1">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="76">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+          <reference field="5" count="1">
+            <x v="10"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="75">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="10"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="73">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" offset="IV256" fieldPosition="0">
+        <references count="1">
+          <reference field="4" count="1">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="71">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+          <reference field="5" count="1">
+            <x v="10"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="69">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="67">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" offset="IV256" fieldPosition="0">
+        <references count="1">
+          <reference field="4" count="1">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="65">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+          <reference field="5" count="1">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="63">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="61">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" offset="IV256" fieldPosition="0">
+        <references count="1">
+          <reference field="4" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="59">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="5" count="1">
+            <x v="9"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="57">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="15"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="55">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" offset="IV256" fieldPosition="0">
+        <references count="1">
+          <reference field="4" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="53">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="5" count="1">
+            <x v="15"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="51">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="12"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="49">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" offset="IV256" fieldPosition="0">
+        <references count="1">
+          <reference field="4" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="47">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1">
+            <x v="12"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
   </formats>
-  <chartFormats count="6">
+  <chartFormats count="3">
     <chartFormat chart="1" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -3699,33 +4367,6 @@
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="7" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="1" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
           </reference>
         </references>
       </pivotArea>
@@ -3737,14 +4378,14 @@
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
     </ext>
     <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
     </ext>
   </extLst>
 </pivotTableDefinition>
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C53DDAB6-DE23-43E4-B3B9-745F13D2F67E}" name="PivotTable2" cacheId="36" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C53DDAB6-DE23-43E4-B3B9-745F13D2F67E}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
   <location ref="A28:B35" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0"/>
@@ -3850,10 +4491,10 @@
     <dataField name="Average of salary_year_avg" fld="2" subtotal="average" baseField="0" baseItem="0" numFmtId="164"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="57">
+    <format dxfId="98">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="58">
+    <format dxfId="97">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -3876,7 +4517,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0DEA7522-070C-4DF9-BD92-1F214C0CED6E}" name="PivotTable1" cacheId="36" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0DEA7522-070C-4DF9-BD92-1F214C0CED6E}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
   <location ref="A3:X11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0"/>
@@ -4054,10 +4695,10 @@
     <dataField name=" salary_year_avg" fld="2" baseField="0" baseItem="0" numFmtId="3"/>
   </dataFields>
   <formats count="19">
-    <format dxfId="77">
+    <format dxfId="117">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="76">
+    <format dxfId="116">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="4" count="1">
@@ -4066,7 +4707,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="38">
+    <format dxfId="115">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="5" count="1">
@@ -4075,7 +4716,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="37">
+    <format dxfId="114">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="5" count="1">
@@ -4084,7 +4725,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="36">
+    <format dxfId="113">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="5" count="1">
@@ -4093,7 +4734,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="35">
+    <format dxfId="112">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="5" count="1">
@@ -4102,7 +4743,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="34">
+    <format dxfId="111">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="5" count="1">
@@ -4111,7 +4752,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="33">
+    <format dxfId="110">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="5" count="1">
@@ -4120,7 +4761,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="32">
+    <format dxfId="109">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="5" count="1">
@@ -4129,7 +4770,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="31">
+    <format dxfId="108">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="5" count="1">
@@ -4138,7 +4779,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="30">
+    <format dxfId="107">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="5" count="1">
@@ -4147,7 +4788,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="29">
+    <format dxfId="106">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="5" count="1">
@@ -4156,7 +4797,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="28">
+    <format dxfId="105">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="5" count="1">
@@ -4165,7 +4806,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="27">
+    <format dxfId="104">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="5" count="1">
@@ -4174,7 +4815,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="26">
+    <format dxfId="103">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="5" count="1">
@@ -4183,7 +4824,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="25">
+    <format dxfId="102">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="5" count="1">
@@ -4192,7 +4833,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="24">
+    <format dxfId="101">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="5" count="1">
@@ -4201,7 +4842,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="23">
+    <format dxfId="100">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="5" count="1">
@@ -4210,7 +4851,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="22">
+    <format dxfId="99">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="5" count="1">
@@ -4233,7 +4874,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A4BBEEF4-F3F7-4822-BAC7-00A68CAA8F29}" name="PivotTable44" cacheId="35" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="7">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A4BBEEF4-F3F7-4822-BAC7-00A68CAA8F29}" name="PivotTable44" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="7">
   <location ref="A3:B21" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -4611,7 +5252,7 @@
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{BE91AAED-C3D4-4E04-8327-B16EA1E507BC}" name="job_id"/>
     <tableColumn id="2" xr3:uid="{D41E2BAE-DD91-4C21-AF07-180F3969AFD6}" name="job_title"/>
-    <tableColumn id="4" xr3:uid="{557BB80A-77BA-480C-8A88-183495055119}" name="job_posted_date" dataDxfId="78"/>
+    <tableColumn id="4" xr3:uid="{557BB80A-77BA-480C-8A88-183495055119}" name="job_posted_date" dataDxfId="118"/>
     <tableColumn id="5" xr3:uid="{61D596F3-05E3-4CD7-857F-A728C059D50B}" name="company_name"/>
     <tableColumn id="3" xr3:uid="{76F8B469-6A63-4388-8EC1-59B6F75292CE}" name="salary_year_avg"/>
     <tableColumn id="6" xr3:uid="{D0682A71-FA52-49C7-9E3B-B014C6A1D806}" name="skills"/>
@@ -5923,18 +6564,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E35335E-3C41-4120-92FF-E3F3CDA15F72}">
-  <dimension ref="A3:X93"/>
+  <dimension ref="A3:X86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="30.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
@@ -6005,64 +6647,64 @@
       <c r="A4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="6" t="s">
         <v>10</v>
       </c>
       <c r="K4" t="s">
         <v>19</v>
       </c>
-      <c r="L4" s="7" t="s">
+      <c r="L4" s="6" t="s">
         <v>16</v>
       </c>
       <c r="M4" t="s">
         <v>18</v>
       </c>
-      <c r="N4" s="7" t="s">
+      <c r="N4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="O4" s="7" t="s">
+      <c r="O4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="P4" s="7" t="s">
+      <c r="P4" s="6" t="s">
         <v>22</v>
       </c>
       <c r="Q4" t="s">
         <v>24</v>
       </c>
-      <c r="R4" s="7" t="s">
+      <c r="R4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="S4" s="7" t="s">
+      <c r="S4" s="6" t="s">
         <v>29</v>
       </c>
       <c r="T4" t="s">
         <v>28</v>
       </c>
-      <c r="U4" s="7" t="s">
+      <c r="U4" s="6" t="s">
         <v>34</v>
       </c>
       <c r="V4" t="s">
@@ -6071,255 +6713,255 @@
       <c r="W4" t="s">
         <v>33</v>
       </c>
-      <c r="X4" s="7" t="s">
+      <c r="X4" s="6" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:24">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>140500</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>140500</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>140500</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>140500</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6">
+      <c r="F5" s="5"/>
+      <c r="G5" s="5">
         <v>140500</v>
       </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6">
+      <c r="H5" s="5"/>
+      <c r="I5" s="5">
         <v>140500</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="5">
         <v>140500</v>
       </c>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6"/>
-      <c r="S5" s="6"/>
-      <c r="T5" s="6"/>
-      <c r="U5" s="6"/>
-      <c r="V5" s="6"/>
-      <c r="W5" s="6"/>
-      <c r="X5" s="6"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5"/>
+      <c r="W5" s="5"/>
+      <c r="X5" s="5"/>
     </row>
     <row r="6" spans="1:24">
       <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>125000</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>125000</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>125000</v>
       </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6">
+      <c r="E6" s="5"/>
+      <c r="F6" s="5">
         <v>250000</v>
       </c>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6">
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5">
         <v>125000</v>
       </c>
-      <c r="L6" s="6">
+      <c r="L6" s="5">
         <v>125000</v>
       </c>
-      <c r="M6" s="6">
+      <c r="M6" s="5">
         <v>125000</v>
       </c>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="6"/>
-      <c r="S6" s="6"/>
-      <c r="T6" s="6"/>
-      <c r="U6" s="6"/>
-      <c r="V6" s="6"/>
-      <c r="W6" s="6"/>
-      <c r="X6" s="6"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
+      <c r="X6" s="5"/>
     </row>
     <row r="7" spans="1:24">
       <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <v>110000</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6">
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5">
         <v>110000</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6">
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5">
         <v>110000</v>
       </c>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6">
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5">
         <v>110000</v>
       </c>
-      <c r="O7" s="6">
+      <c r="O7" s="5">
         <v>110000</v>
       </c>
-      <c r="P7" s="6">
+      <c r="P7" s="5">
         <v>110000</v>
       </c>
-      <c r="Q7" s="6">
+      <c r="Q7" s="5">
         <v>110000</v>
       </c>
-      <c r="R7" s="6"/>
-      <c r="S7" s="6"/>
-      <c r="T7" s="6"/>
-      <c r="U7" s="6"/>
-      <c r="V7" s="6"/>
-      <c r="W7" s="6"/>
-      <c r="X7" s="6"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5"/>
+      <c r="W7" s="5"/>
+      <c r="X7" s="5"/>
     </row>
     <row r="8" spans="1:24">
       <c r="A8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <v>105000</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>105000</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>105000</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>105000</v>
       </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6">
+      <c r="F8" s="5"/>
+      <c r="G8" s="5">
         <v>105000</v>
       </c>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="6">
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5">
         <v>105000</v>
       </c>
-      <c r="S8" s="6">
+      <c r="S8" s="5">
         <v>105000</v>
       </c>
-      <c r="T8" s="6">
+      <c r="T8" s="5">
         <v>105000</v>
       </c>
-      <c r="U8" s="6"/>
-      <c r="V8" s="6"/>
-      <c r="W8" s="6"/>
-      <c r="X8" s="6"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="5"/>
+      <c r="W8" s="5"/>
+      <c r="X8" s="5"/>
     </row>
     <row r="9" spans="1:24">
       <c r="A9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <v>102250</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>102250</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6"/>
-      <c r="R9" s="6"/>
-      <c r="S9" s="6"/>
-      <c r="T9" s="6"/>
-      <c r="U9" s="6"/>
-      <c r="V9" s="6"/>
-      <c r="W9" s="6"/>
-      <c r="X9" s="6"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="5"/>
+      <c r="X9" s="5"/>
     </row>
     <row r="10" spans="1:24">
       <c r="A10" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <v>78000</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <v>78000</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="5">
         <v>78000</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <v>78000</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="5">
         <v>156000</v>
       </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="6"/>
-      <c r="S10" s="6"/>
-      <c r="T10" s="6"/>
-      <c r="U10" s="6">
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="5"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="5">
         <v>78000</v>
       </c>
-      <c r="V10" s="6">
+      <c r="V10" s="5">
         <v>78000</v>
       </c>
-      <c r="W10" s="6">
+      <c r="W10" s="5">
         <v>78000</v>
       </c>
-      <c r="X10" s="6">
+      <c r="X10" s="5">
         <v>78000</v>
       </c>
     </row>
@@ -6327,46 +6969,46 @@
       <c r="A11" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="5">
         <v>70000</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <v>70000</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="5">
         <v>70000</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6">
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5">
         <v>70000</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="5">
         <v>70000</v>
       </c>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="6"/>
-      <c r="S11" s="6"/>
-      <c r="T11" s="6"/>
-      <c r="U11" s="6"/>
-      <c r="V11" s="6"/>
-      <c r="W11" s="6"/>
-      <c r="X11" s="6"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="5"/>
+      <c r="V11" s="5"/>
+      <c r="W11" s="5"/>
+      <c r="X11" s="5"/>
     </row>
     <row r="16" spans="1:24">
       <c r="A16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>42</v>
+      <c r="B16" s="6" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -6429,15 +7071,15 @@
       <c r="A28" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="7" t="s">
-        <v>41</v>
+      <c r="B28" s="6" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B29" s="9">
+      <c r="B29" s="8">
         <v>140500</v>
       </c>
     </row>
@@ -6445,7 +7087,7 @@
       <c r="A30" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="9">
+      <c r="B30" s="8">
         <v>125000</v>
       </c>
     </row>
@@ -6453,7 +7095,7 @@
       <c r="A31" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="9">
+      <c r="B31" s="8">
         <v>110000</v>
       </c>
     </row>
@@ -6461,7 +7103,7 @@
       <c r="A32" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B32" s="9">
+      <c r="B32" s="8">
         <v>105000</v>
       </c>
     </row>
@@ -6469,7 +7111,7 @@
       <c r="A33" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="9">
+      <c r="B33" s="8">
         <v>102250</v>
       </c>
     </row>
@@ -6477,7 +7119,7 @@
       <c r="A34" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B34" s="9">
+      <c r="B34" s="8">
         <v>78000</v>
       </c>
     </row>
@@ -6485,577 +7127,407 @@
       <c r="A35" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B35" s="9">
+      <c r="B35" s="8">
         <v>70000</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B41" t="s">
-        <v>41</v>
-      </c>
-      <c r="C41" t="s">
-        <v>40</v>
+        <v>42</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="3" t="s">
+      <c r="A42" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="6">
+      <c r="B42" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" s="8">
         <v>140500</v>
       </c>
-      <c r="C42" s="4"/>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="5" t="s">
+      <c r="B43" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43" s="8">
+        <v>140500</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="B44" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" s="8">
+        <v>140500</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="B45" t="s">
+        <v>10</v>
+      </c>
+      <c r="C45" s="8">
+        <v>140500</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="B46" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" s="8">
+        <v>140500</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="B47" t="s">
+        <v>12</v>
+      </c>
+      <c r="C47" s="8">
+        <v>140500</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="9"/>
+      <c r="B48" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C48" s="10">
+        <v>140500</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>15</v>
+      </c>
+      <c r="B49" t="s">
+        <v>19</v>
+      </c>
+      <c r="C49" s="8">
+        <v>125000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="B50" t="s">
+        <v>16</v>
+      </c>
+      <c r="C50" s="8">
+        <v>125000</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="B51" t="s">
+        <v>18</v>
+      </c>
+      <c r="C51" s="8">
+        <v>125000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="B52" t="s">
+        <v>12</v>
+      </c>
+      <c r="C52" s="8">
+        <v>125000</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="B53" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53" s="8">
+        <v>125000</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="B54" t="s">
+        <v>13</v>
+      </c>
+      <c r="C54" s="8">
+        <v>125000</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="9"/>
+      <c r="B55" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C55" s="10">
+        <v>125000</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
+        <v>20</v>
+      </c>
+      <c r="B56" t="s">
+        <v>22</v>
+      </c>
+      <c r="C56" s="8">
+        <v>110000</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="B57" t="s">
+        <v>21</v>
+      </c>
+      <c r="C57" s="8">
+        <v>110000</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="B58" t="s">
+        <v>24</v>
+      </c>
+      <c r="C58" s="8">
+        <v>110000</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="B59" t="s">
         <v>8</v>
       </c>
-      <c r="B43" s="6">
-        <v>140500</v>
-      </c>
-      <c r="C43" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B44" s="6">
-        <v>140500</v>
-      </c>
-      <c r="C44" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="5" t="s">
+      <c r="C59" s="8">
+        <v>110000</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="B60" t="s">
+        <v>25</v>
+      </c>
+      <c r="C60" s="8">
+        <v>110000</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="B61" t="s">
+        <v>23</v>
+      </c>
+      <c r="C61" s="8">
+        <v>110000</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="9"/>
+      <c r="B62" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B45" s="6">
-        <v>140500</v>
-      </c>
-      <c r="C45" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B46" s="6">
-        <v>140500</v>
-      </c>
-      <c r="C46" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="5" t="s">
+      <c r="C62" s="10">
+        <v>110000</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
+        <v>26</v>
+      </c>
+      <c r="B63" t="s">
         <v>9</v>
       </c>
-      <c r="B47" s="6">
-        <v>140500</v>
-      </c>
-      <c r="C47" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="5" t="s">
+      <c r="C63" s="8">
+        <v>105000</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="B64" t="s">
+        <v>28</v>
+      </c>
+      <c r="C64" s="8">
+        <v>105000</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="B65" t="s">
+        <v>13</v>
+      </c>
+      <c r="C65" s="8">
+        <v>105000</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="B66" t="s">
+        <v>8</v>
+      </c>
+      <c r="C66" s="8">
+        <v>105000</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="B67" t="s">
+        <v>11</v>
+      </c>
+      <c r="C67" s="8">
+        <v>105000</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="B68" t="s">
         <v>12</v>
       </c>
-      <c r="B48" s="6">
-        <v>140500</v>
-      </c>
-      <c r="C48" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="5" t="s">
+      <c r="C68" s="8">
+        <v>105000</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="B69" t="s">
+        <v>27</v>
+      </c>
+      <c r="C69" s="8">
+        <v>105000</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="9"/>
+      <c r="B70" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C70" s="10">
+        <v>105000</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" t="s">
+        <v>30</v>
+      </c>
+      <c r="B71" t="s">
+        <v>11</v>
+      </c>
+      <c r="C71" s="8">
+        <v>102250</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="9"/>
+      <c r="B72" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C72" s="10">
+        <v>102250</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" t="s">
+        <v>31</v>
+      </c>
+      <c r="B73" t="s">
+        <v>32</v>
+      </c>
+      <c r="C73" s="8">
+        <v>78000</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="B74" t="s">
+        <v>17</v>
+      </c>
+      <c r="C74" s="8">
+        <v>78000</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="B75" t="s">
+        <v>35</v>
+      </c>
+      <c r="C75" s="8">
+        <v>78000</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="B76" t="s">
+        <v>8</v>
+      </c>
+      <c r="C76" s="8">
+        <v>78000</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="B77" t="s">
+        <v>11</v>
+      </c>
+      <c r="C77" s="8">
+        <v>78000</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="B78" t="s">
+        <v>33</v>
+      </c>
+      <c r="C78" s="8">
+        <v>78000</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="B79" t="s">
+        <v>34</v>
+      </c>
+      <c r="C79" s="8">
+        <v>78000</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="B80" t="s">
+        <v>12</v>
+      </c>
+      <c r="C80" s="8">
+        <v>78000</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="9"/>
+      <c r="B81" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B49" s="6">
-        <v>140500</v>
-      </c>
-      <c r="C49" s="4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B50" s="6">
-        <v>125000</v>
-      </c>
-      <c r="C50" s="4"/>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B51" s="6">
-        <v>125000</v>
-      </c>
-      <c r="C51" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B52" s="6">
-        <v>125000</v>
-      </c>
-      <c r="C52" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B53" s="6">
-        <v>125000</v>
-      </c>
-      <c r="C53" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" s="5" t="s">
+      <c r="C81" s="10">
+        <v>78000</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" t="s">
+        <v>36</v>
+      </c>
+      <c r="B82" t="s">
+        <v>11</v>
+      </c>
+      <c r="C82" s="8">
+        <v>70000</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="B83" t="s">
+        <v>23</v>
+      </c>
+      <c r="C83" s="8">
+        <v>70000</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="B84" t="s">
+        <v>9</v>
+      </c>
+      <c r="C84" s="8">
+        <v>70000</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="B85" t="s">
         <v>12</v>
       </c>
-      <c r="B54" s="6">
-        <v>125000</v>
-      </c>
-      <c r="C54" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B55" s="6">
-        <v>125000</v>
-      </c>
-      <c r="C55" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="A56" s="5" t="s">
+      <c r="C85" s="8">
+        <v>70000</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" s="9"/>
+      <c r="B86" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B56" s="6">
-        <v>125000</v>
-      </c>
-      <c r="C56" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B57" s="6">
-        <v>125000</v>
-      </c>
-      <c r="C57" s="4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B58" s="6">
-        <v>110000</v>
-      </c>
-      <c r="C58" s="4"/>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B59" s="6">
-        <v>110000</v>
-      </c>
-      <c r="C59" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B60" s="6">
-        <v>110000</v>
-      </c>
-      <c r="C60" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B61" s="6">
-        <v>110000</v>
-      </c>
-      <c r="C61" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="A62" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B62" s="6">
-        <v>110000</v>
-      </c>
-      <c r="C62" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="A63" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B63" s="6">
-        <v>110000</v>
-      </c>
-      <c r="C63" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="A64" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B64" s="6">
-        <v>110000</v>
-      </c>
-      <c r="C64" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B65" s="6">
-        <v>110000</v>
-      </c>
-      <c r="C65" s="4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B66" s="6">
-        <v>105000</v>
-      </c>
-      <c r="C66" s="4"/>
-    </row>
-    <row r="67" spans="1:3">
-      <c r="A67" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B67" s="6">
-        <v>105000</v>
-      </c>
-      <c r="C67" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3">
-      <c r="A68" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B68" s="6">
-        <v>105000</v>
-      </c>
-      <c r="C68" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B69" s="6">
-        <v>105000</v>
-      </c>
-      <c r="C69" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3">
-      <c r="A70" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B70" s="6">
-        <v>105000</v>
-      </c>
-      <c r="C70" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3">
-      <c r="A71" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B71" s="6">
-        <v>105000</v>
-      </c>
-      <c r="C71" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3">
-      <c r="A72" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B72" s="6">
-        <v>105000</v>
-      </c>
-      <c r="C72" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
-      <c r="A73" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B73" s="6">
-        <v>105000</v>
-      </c>
-      <c r="C73" s="4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="A74" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B74" s="6">
-        <v>105000</v>
-      </c>
-      <c r="C74" s="4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3">
-      <c r="A75" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B75" s="6">
-        <v>102250</v>
-      </c>
-      <c r="C75" s="4"/>
-    </row>
-    <row r="76" spans="1:3">
-      <c r="A76" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B76" s="6">
-        <v>102250</v>
-      </c>
-      <c r="C76" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3">
-      <c r="A77" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B77" s="6">
-        <v>102250</v>
-      </c>
-      <c r="C77" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3">
-      <c r="A78" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B78" s="6">
-        <v>78000</v>
-      </c>
-      <c r="C78" s="4"/>
-    </row>
-    <row r="79" spans="1:3">
-      <c r="A79" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B79" s="6">
-        <v>78000</v>
-      </c>
-      <c r="C79" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3">
-      <c r="A80" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B80" s="6">
-        <v>78000</v>
-      </c>
-      <c r="C80" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3">
-      <c r="A81" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B81" s="6">
-        <v>78000</v>
-      </c>
-      <c r="C81" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3">
-      <c r="A82" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B82" s="6">
-        <v>78000</v>
-      </c>
-      <c r="C82" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3">
-      <c r="A83" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B83" s="6">
-        <v>78000</v>
-      </c>
-      <c r="C83" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3">
-      <c r="A84" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B84" s="6">
-        <v>78000</v>
-      </c>
-      <c r="C84" s="4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3">
-      <c r="A85" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B85" s="6">
-        <v>78000</v>
-      </c>
-      <c r="C85" s="4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3">
-      <c r="A86" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B86" s="6">
-        <v>78000</v>
-      </c>
-      <c r="C86" s="4">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3">
-      <c r="A87" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B87" s="6">
-        <v>78000</v>
-      </c>
-      <c r="C87" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3">
-      <c r="A88" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B88" s="6">
+      <c r="C86" s="10">
         <v>70000</v>
-      </c>
-      <c r="C88" s="4"/>
-    </row>
-    <row r="89" spans="1:3">
-      <c r="A89" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B89" s="6">
-        <v>70000</v>
-      </c>
-      <c r="C89" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3">
-      <c r="A90" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B90" s="6">
-        <v>70000</v>
-      </c>
-      <c r="C90" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3">
-      <c r="A91" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B91" s="6">
-        <v>70000</v>
-      </c>
-      <c r="C91" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3">
-      <c r="A92" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B92" s="6">
-        <v>70000</v>
-      </c>
-      <c r="C92" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3">
-      <c r="A93" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B93" s="6">
-        <v>70000</v>
-      </c>
-      <c r="C93" s="4">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -7096,7 +7568,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:2">

</xml_diff>